<commit_message>
Add numbers of the rules
</commit_message>
<xml_diff>
--- a/final_method/分析表.xlsx
+++ b/final_method/分析表.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\user\source\repos\Compiler\final_method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E25ABAC-09B9-4C2D-8AA0-3886C18B5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6969B7-CFEF-4082-8043-8DF7DFED6AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{85660D98-9A17-4E4E-93F8-C6FB2685D6EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{85660D98-9A17-4E4E-93F8-C6FB2685D6EB}"/>
   </bookViews>
   <sheets>
     <sheet name="LALR(1)分析表" sheetId="4" r:id="rId1"/>
     <sheet name="非终结符说明" sheetId="5" r:id="rId2"/>
+    <sheet name="语法规则编号" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="257">
   <si>
     <t>acc</t>
   </si>
@@ -1250,6 +1251,174 @@
       <t>r16</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P -&gt; program f ; Q M .</t>
+  </si>
+  <si>
+    <t>T -&gt; integer</t>
+  </si>
+  <si>
+    <t>T -&gt; bool</t>
+  </si>
+  <si>
+    <t>T -&gt; char</t>
+  </si>
+  <si>
+    <t>X -&gt; A</t>
+  </si>
+  <si>
+    <t>X -&gt; B</t>
+  </si>
+  <si>
+    <t>X -&gt; C</t>
+  </si>
+  <si>
+    <t>A -&gt; A + I</t>
+  </si>
+  <si>
+    <t>A -&gt; A - I</t>
+  </si>
+  <si>
+    <t>A -&gt; I</t>
+  </si>
+  <si>
+    <t>I -&gt; I * F</t>
+  </si>
+  <si>
+    <t>I -&gt; I / F</t>
+  </si>
+  <si>
+    <t>I -&gt; F</t>
+  </si>
+  <si>
+    <t>F -&gt; V</t>
+  </si>
+  <si>
+    <t>F -&gt; - F</t>
+  </si>
+  <si>
+    <t>V -&gt; i</t>
+  </si>
+  <si>
+    <t>V -&gt; f</t>
+  </si>
+  <si>
+    <t>V -&gt; ( A )</t>
+  </si>
+  <si>
+    <t>B -&gt; B or J</t>
+  </si>
+  <si>
+    <t>B -&gt; J</t>
+  </si>
+  <si>
+    <t>J -&gt; J and G</t>
+  </si>
+  <si>
+    <t>J -&gt; G</t>
+  </si>
+  <si>
+    <t>G -&gt; U</t>
+  </si>
+  <si>
+    <t>G -&gt; not G</t>
+  </si>
+  <si>
+    <t>U -&gt; w</t>
+  </si>
+  <si>
+    <t>U -&gt; f</t>
+  </si>
+  <si>
+    <t>U -&gt; ( B )</t>
+  </si>
+  <si>
+    <t>U -&gt; f R f</t>
+  </si>
+  <si>
+    <t>U -&gt; A R A</t>
+  </si>
+  <si>
+    <t>R -&gt; &lt;</t>
+  </si>
+  <si>
+    <t>R -&gt; &lt;&gt;</t>
+  </si>
+  <si>
+    <t>R -&gt; &lt;=</t>
+  </si>
+  <si>
+    <t>R -&gt; &gt;=</t>
+  </si>
+  <si>
+    <t>R -&gt; &gt;</t>
+  </si>
+  <si>
+    <t>R -&gt; =</t>
+  </si>
+  <si>
+    <t>C -&gt; t</t>
+  </si>
+  <si>
+    <t>C -&gt; f</t>
+  </si>
+  <si>
+    <t>S -&gt; E</t>
+  </si>
+  <si>
+    <t>S -&gt; IF_S</t>
+  </si>
+  <si>
+    <t>S -&gt; WHILE_S</t>
+  </si>
+  <si>
+    <t>S -&gt; REPEAT_S</t>
+  </si>
+  <si>
+    <t>S -&gt; M</t>
+  </si>
+  <si>
+    <t>E -&gt; f := X</t>
+  </si>
+  <si>
+    <t>IF_S -&gt; if B then S</t>
+  </si>
+  <si>
+    <t>IF_S -&gt; if B then S else S</t>
+  </si>
+  <si>
+    <t>WHILE_S -&gt; while B do S</t>
+  </si>
+  <si>
+    <t>REPEAT_S -&gt; repeat S until B</t>
+  </si>
+  <si>
+    <t>M -&gt; begin L end</t>
+  </si>
+  <si>
+    <t>L -&gt; S ; L</t>
+  </si>
+  <si>
+    <t>L -&gt; S</t>
+  </si>
+  <si>
+    <t>Q -&gt; var D</t>
+  </si>
+  <si>
+    <t>Q -&gt; ''</t>
+  </si>
+  <si>
+    <t>D -&gt; O : T ; D</t>
+  </si>
+  <si>
+    <t>D -&gt; O : T ;</t>
+  </si>
+  <si>
+    <t>O -&gt; f , O</t>
+  </si>
+  <si>
+    <t>O -&gt; f</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1481,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1372,24 +1541,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1398,6 +1570,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1717,79 +1898,79 @@
   <sheetPr codeName="工作表2"/>
   <dimension ref="A2:BK100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="BJ16" sqref="BJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5"/>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5"/>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="5"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5"/>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5"/>
-      <c r="BJ2" s="5"/>
-      <c r="BK2" s="5"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="3"/>
+      <c r="AW2" s="3"/>
+      <c r="AX2" s="3"/>
+      <c r="AY2" s="3"/>
+      <c r="AZ2" s="3"/>
+      <c r="BA2" s="3"/>
+      <c r="BB2" s="3"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
+      <c r="BI2" s="3"/>
+      <c r="BJ2" s="3"/>
+      <c r="BK2" s="3"/>
     </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -9949,8 +10130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974DB324-053D-4CBB-BDC5-65D49E568C61}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -9959,127 +10140,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="5" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>167</v>
       </c>
     </row>
@@ -10088,4 +10269,639 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3551D49-187C-4829-9BA5-46F59B673A80}">
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="56">
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add arithmetic expression semantic analysis
</commit_message>
<xml_diff>
--- a/final_method/分析表.xlsx
+++ b/final_method/分析表.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\user\source\repos\Compiler\final_method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BACEF2-A059-482C-AE16-53441C0771C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB36B6B6-1016-41D1-B790-A34ABA5BF3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{85660D98-9A17-4E4E-93F8-C6FB2685D6EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{85660D98-9A17-4E4E-93F8-C6FB2685D6EB}"/>
   </bookViews>
   <sheets>
     <sheet name="LALR(1)分析表" sheetId="4" r:id="rId1"/>
-    <sheet name="非终结符说明" sheetId="5" r:id="rId2"/>
-    <sheet name="语法规则编号" sheetId="6" r:id="rId3"/>
+    <sheet name="Decide" sheetId="7" r:id="rId2"/>
+    <sheet name="非终结符说明" sheetId="5" r:id="rId3"/>
+    <sheet name="语法规则编号" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LALR(1)分析表'!$A$3:$BK$100</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="260">
   <si>
     <t>acc</t>
   </si>
@@ -1345,12 +1346,27 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>d1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>r33/r13/r22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>r22/r13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1501,7 +1517,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1533,6 +1549,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1852,13 +1871,13 @@
   <sheetPr codeName="工作表2"/>
   <dimension ref="A2:BM101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="E73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG67" sqref="AG67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <sheetData>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:65">
       <c r="B2" s="6" t="s">
         <v>111</v>
       </c>
@@ -1927,7 +1946,7 @@
       <c r="BK2" s="7"/>
       <c r="BL2" s="7"/>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2118,7 +2137,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -2189,7 +2208,7 @@
       <c r="BL4" s="4"/>
       <c r="BM4" s="5"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -2260,7 +2279,7 @@
       <c r="BL5" s="4"/>
       <c r="BM5" s="5"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -2331,7 +2350,7 @@
       <c r="BL6" s="4"/>
       <c r="BM6" s="5"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -2406,7 +2425,7 @@
       <c r="BL7" s="4"/>
       <c r="BM7" s="5"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -2479,7 +2498,7 @@
       <c r="BL8" s="4"/>
       <c r="BM8" s="5"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -2554,7 +2573,7 @@
       </c>
       <c r="BM9" s="5"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -2625,7 +2644,7 @@
       <c r="BL10" s="4"/>
       <c r="BM10" s="5"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -2722,7 +2741,7 @@
       <c r="BL11" s="4"/>
       <c r="BM11" s="5"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -2793,7 +2812,7 @@
       <c r="BL12" s="4"/>
       <c r="BM12" s="5"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -2864,7 +2883,7 @@
       <c r="BL13" s="4"/>
       <c r="BM13" s="5"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -2937,7 +2956,7 @@
       <c r="BL14" s="4"/>
       <c r="BM14" s="5"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:65">
       <c r="A15" s="4">
         <v>11</v>
       </c>
@@ -3008,7 +3027,7 @@
       <c r="BL15" s="4"/>
       <c r="BM15" s="5"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:65">
       <c r="A16" s="4">
         <v>12</v>
       </c>
@@ -3081,7 +3100,7 @@
       <c r="BL16" s="4"/>
       <c r="BM16" s="5"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65">
       <c r="A17" s="4">
         <v>13</v>
       </c>
@@ -3174,7 +3193,7 @@
       <c r="BL17" s="4"/>
       <c r="BM17" s="5"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -3247,7 +3266,7 @@
       <c r="BL18" s="4"/>
       <c r="BM18" s="5"/>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65">
       <c r="A19" s="4">
         <v>15</v>
       </c>
@@ -3324,7 +3343,7 @@
       <c r="BL19" s="4"/>
       <c r="BM19" s="5"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:65">
       <c r="A20" s="4">
         <v>16</v>
       </c>
@@ -3401,7 +3420,7 @@
       <c r="BL20" s="4"/>
       <c r="BM20" s="5"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:65">
       <c r="A21" s="4">
         <v>17</v>
       </c>
@@ -3494,7 +3513,7 @@
       <c r="BL21" s="4"/>
       <c r="BM21" s="5"/>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65">
       <c r="A22" s="4">
         <v>18</v>
       </c>
@@ -3587,7 +3606,7 @@
       <c r="BL22" s="4"/>
       <c r="BM22" s="5"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:65">
       <c r="A23" s="4">
         <v>19</v>
       </c>
@@ -3680,7 +3699,7 @@
       <c r="BL23" s="4"/>
       <c r="BM23" s="5"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:65">
       <c r="A24" s="4">
         <v>20</v>
       </c>
@@ -3773,7 +3792,7 @@
       <c r="BL24" s="4"/>
       <c r="BM24" s="5"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:65">
       <c r="A25" s="4">
         <v>21</v>
       </c>
@@ -3844,7 +3863,7 @@
       <c r="BL25" s="4"/>
       <c r="BM25" s="5"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:65">
       <c r="A26" s="4">
         <v>22</v>
       </c>
@@ -3941,7 +3960,7 @@
       <c r="BL26" s="4"/>
       <c r="BM26" s="5"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:65">
       <c r="A27" s="4">
         <v>23</v>
       </c>
@@ -4014,7 +4033,7 @@
       <c r="BL27" s="4"/>
       <c r="BM27" s="5"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:65">
       <c r="A28" s="4">
         <v>24</v>
       </c>
@@ -4085,7 +4104,7 @@
       <c r="BL28" s="4"/>
       <c r="BM28" s="5"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:65">
       <c r="A29" s="4">
         <v>25</v>
       </c>
@@ -4162,7 +4181,7 @@
       </c>
       <c r="BM29" s="5"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:65">
       <c r="A30" s="4">
         <v>26</v>
       </c>
@@ -4235,7 +4254,7 @@
       </c>
       <c r="BM30" s="5"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:65">
       <c r="A31" s="4">
         <v>27</v>
       </c>
@@ -4310,7 +4329,7 @@
       <c r="BL31" s="4"/>
       <c r="BM31" s="5"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:65">
       <c r="A32" s="4">
         <v>28</v>
       </c>
@@ -4389,7 +4408,7 @@
       <c r="BL32" s="4"/>
       <c r="BM32" s="5"/>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:65">
       <c r="A33" s="4">
         <v>29</v>
       </c>
@@ -4468,7 +4487,7 @@
       <c r="BL33" s="4"/>
       <c r="BM33" s="5"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:65">
       <c r="A34" s="4">
         <v>30</v>
       </c>
@@ -4541,7 +4560,7 @@
       <c r="BL34" s="4"/>
       <c r="BM34" s="5"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:65">
       <c r="A35" s="4">
         <v>31</v>
       </c>
@@ -4618,7 +4637,7 @@
       <c r="BL35" s="4"/>
       <c r="BM35" s="5"/>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:65">
       <c r="A36" s="4">
         <v>32</v>
       </c>
@@ -4695,7 +4714,7 @@
       <c r="BL36" s="4"/>
       <c r="BM36" s="5"/>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:65">
       <c r="A37" s="4">
         <v>33</v>
       </c>
@@ -4772,7 +4791,7 @@
       <c r="BL37" s="4"/>
       <c r="BM37" s="5"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:65">
       <c r="A38" s="4">
         <v>34</v>
       </c>
@@ -4843,7 +4862,7 @@
       <c r="BL38" s="4"/>
       <c r="BM38" s="5"/>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:65">
       <c r="A39" s="4">
         <v>35</v>
       </c>
@@ -4946,7 +4965,7 @@
       <c r="BL39" s="4"/>
       <c r="BM39" s="5"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:65">
       <c r="A40" s="4">
         <v>36</v>
       </c>
@@ -5019,7 +5038,7 @@
       <c r="BL40" s="4"/>
       <c r="BM40" s="5"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:65">
       <c r="A41" s="4">
         <v>37</v>
       </c>
@@ -5106,7 +5125,7 @@
       <c r="BL41" s="4"/>
       <c r="BM41" s="5"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:65">
       <c r="A42" s="4">
         <v>38</v>
       </c>
@@ -5193,7 +5212,7 @@
       <c r="BL42" s="4"/>
       <c r="BM42" s="5"/>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:65">
       <c r="A43" s="4">
         <v>39</v>
       </c>
@@ -5280,7 +5299,7 @@
       <c r="BL43" s="4"/>
       <c r="BM43" s="5"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:65">
       <c r="A44" s="4">
         <v>40</v>
       </c>
@@ -5373,7 +5392,7 @@
       <c r="BL44" s="4"/>
       <c r="BM44" s="5"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:65">
       <c r="A45" s="4">
         <v>41</v>
       </c>
@@ -5460,7 +5479,7 @@
       <c r="BL45" s="4"/>
       <c r="BM45" s="5"/>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:65">
       <c r="A46" s="4">
         <v>42</v>
       </c>
@@ -5569,7 +5588,7 @@
       <c r="BL46" s="4"/>
       <c r="BM46" s="5"/>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:65">
       <c r="A47" s="4">
         <v>43</v>
       </c>
@@ -5666,7 +5685,7 @@
       <c r="BL47" s="4"/>
       <c r="BM47" s="5"/>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:65">
       <c r="A48" s="4">
         <v>44</v>
       </c>
@@ -5753,7 +5772,7 @@
       <c r="BL48" s="4"/>
       <c r="BM48" s="5"/>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:65">
       <c r="A49" s="4">
         <v>45</v>
       </c>
@@ -5860,7 +5879,7 @@
       <c r="BL49" s="4"/>
       <c r="BM49" s="5"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:65">
       <c r="A50" s="4">
         <v>46</v>
       </c>
@@ -5967,7 +5986,7 @@
       <c r="BL50" s="4"/>
       <c r="BM50" s="5"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:65">
       <c r="A51" s="4">
         <v>47</v>
       </c>
@@ -6074,7 +6093,7 @@
       <c r="BL51" s="4"/>
       <c r="BM51" s="5"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:65">
       <c r="A52" s="4">
         <v>48</v>
       </c>
@@ -6155,7 +6174,7 @@
       <c r="BL52" s="4"/>
       <c r="BM52" s="5"/>
     </row>
-    <row r="53" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:65">
       <c r="A53" s="4">
         <v>49</v>
       </c>
@@ -6262,7 +6281,7 @@
       <c r="BL53" s="4"/>
       <c r="BM53" s="5"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:65">
       <c r="A54" s="4">
         <v>50</v>
       </c>
@@ -6333,7 +6352,7 @@
       <c r="BL54" s="4"/>
       <c r="BM54" s="5"/>
     </row>
-    <row r="55" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:65">
       <c r="A55" s="4">
         <v>51</v>
       </c>
@@ -6404,7 +6423,7 @@
       <c r="BL55" s="4"/>
       <c r="BM55" s="5"/>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:65">
       <c r="A56" s="4">
         <v>52</v>
       </c>
@@ -6475,7 +6494,7 @@
       <c r="BL56" s="4"/>
       <c r="BM56" s="5"/>
     </row>
-    <row r="57" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:65">
       <c r="A57" s="4">
         <v>53</v>
       </c>
@@ -6546,7 +6565,7 @@
       <c r="BL57" s="4"/>
       <c r="BM57" s="5"/>
     </row>
-    <row r="58" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:65">
       <c r="A58" s="4">
         <v>54</v>
       </c>
@@ -6617,7 +6636,7 @@
       <c r="BL58" s="4"/>
       <c r="BM58" s="5"/>
     </row>
-    <row r="59" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:65">
       <c r="A59" s="4">
         <v>55</v>
       </c>
@@ -6688,7 +6707,7 @@
       <c r="BL59" s="4"/>
       <c r="BM59" s="5"/>
     </row>
-    <row r="60" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:65">
       <c r="A60" s="4">
         <v>56</v>
       </c>
@@ -6767,7 +6786,7 @@
       <c r="BL60" s="4"/>
       <c r="BM60" s="5"/>
     </row>
-    <row r="61" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:65">
       <c r="A61" s="4">
         <v>57</v>
       </c>
@@ -6864,7 +6883,7 @@
       <c r="BL61" s="4"/>
       <c r="BM61" s="5"/>
     </row>
-    <row r="62" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:65">
       <c r="A62" s="4">
         <v>58</v>
       </c>
@@ -6943,7 +6962,7 @@
       <c r="BL62" s="4"/>
       <c r="BM62" s="5"/>
     </row>
-    <row r="63" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:65">
       <c r="A63" s="4">
         <v>59</v>
       </c>
@@ -7040,7 +7059,7 @@
       <c r="BL63" s="4"/>
       <c r="BM63" s="5"/>
     </row>
-    <row r="64" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:65">
       <c r="A64" s="4">
         <v>60</v>
       </c>
@@ -7121,7 +7140,7 @@
       <c r="BL64" s="4"/>
       <c r="BM64" s="5"/>
     </row>
-    <row r="65" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:65">
       <c r="A65" s="4">
         <v>61</v>
       </c>
@@ -7200,7 +7219,7 @@
       <c r="BL65" s="4"/>
       <c r="BM65" s="5"/>
     </row>
-    <row r="66" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:65">
       <c r="A66" s="4">
         <v>62</v>
       </c>
@@ -7279,7 +7298,7 @@
       <c r="BL66" s="4"/>
       <c r="BM66" s="5"/>
     </row>
-    <row r="67" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:65">
       <c r="A67" s="4">
         <v>63</v>
       </c>
@@ -7384,7 +7403,7 @@
       <c r="BL67" s="4"/>
       <c r="BM67" s="5"/>
     </row>
-    <row r="68" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:65">
       <c r="A68" s="4">
         <v>64</v>
       </c>
@@ -7463,7 +7482,7 @@
       <c r="BL68" s="4"/>
       <c r="BM68" s="5"/>
     </row>
-    <row r="69" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:65">
       <c r="A69" s="4">
         <v>65</v>
       </c>
@@ -7558,7 +7577,7 @@
       <c r="BL69" s="4"/>
       <c r="BM69" s="5"/>
     </row>
-    <row r="70" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:65">
       <c r="A70" s="4">
         <v>66</v>
       </c>
@@ -7651,7 +7670,7 @@
       <c r="BL70" s="4"/>
       <c r="BM70" s="5"/>
     </row>
-    <row r="71" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:65">
       <c r="A71" s="4">
         <v>67</v>
       </c>
@@ -7738,7 +7757,7 @@
       <c r="BL71" s="4"/>
       <c r="BM71" s="5"/>
     </row>
-    <row r="72" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:65">
       <c r="A72" s="4">
         <v>68</v>
       </c>
@@ -7809,7 +7828,7 @@
       <c r="BL72" s="4"/>
       <c r="BM72" s="5"/>
     </row>
-    <row r="73" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:65">
       <c r="A73" s="4">
         <v>69</v>
       </c>
@@ -7886,7 +7905,7 @@
       <c r="BL73" s="4"/>
       <c r="BM73" s="5"/>
     </row>
-    <row r="74" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:65">
       <c r="A74" s="4">
         <v>70</v>
       </c>
@@ -7963,7 +7982,7 @@
       <c r="BL74" s="4"/>
       <c r="BM74" s="5"/>
     </row>
-    <row r="75" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:65">
       <c r="A75" s="4">
         <v>71</v>
       </c>
@@ -8040,7 +8059,7 @@
       <c r="BL75" s="4"/>
       <c r="BM75" s="5"/>
     </row>
-    <row r="76" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:65">
       <c r="A76" s="4">
         <v>72</v>
       </c>
@@ -8117,7 +8136,7 @@
       <c r="BL76" s="4"/>
       <c r="BM76" s="5"/>
     </row>
-    <row r="77" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:65">
       <c r="A77" s="4">
         <v>73</v>
       </c>
@@ -8194,7 +8213,7 @@
       <c r="BL77" s="4"/>
       <c r="BM77" s="5"/>
     </row>
-    <row r="78" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:65">
       <c r="A78" s="4">
         <v>74</v>
       </c>
@@ -8271,7 +8290,7 @@
       <c r="BL78" s="4"/>
       <c r="BM78" s="5"/>
     </row>
-    <row r="79" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:65">
       <c r="A79" s="4">
         <v>75</v>
       </c>
@@ -8344,7 +8363,7 @@
       <c r="BL79" s="4"/>
       <c r="BM79" s="5"/>
     </row>
-    <row r="80" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:65">
       <c r="A80" s="4">
         <v>76</v>
       </c>
@@ -8433,7 +8452,7 @@
       <c r="BL80" s="4"/>
       <c r="BM80" s="5"/>
     </row>
-    <row r="81" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:65">
       <c r="A81" s="4">
         <v>77</v>
       </c>
@@ -8518,7 +8537,7 @@
       <c r="BL81" s="4"/>
       <c r="BM81" s="5"/>
     </row>
-    <row r="82" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:65">
       <c r="A82" s="4">
         <v>78</v>
       </c>
@@ -8601,7 +8620,7 @@
       <c r="BL82" s="4"/>
       <c r="BM82" s="5"/>
     </row>
-    <row r="83" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:65">
       <c r="A83" s="4">
         <v>79</v>
       </c>
@@ -8684,7 +8703,7 @@
       <c r="BL83" s="4"/>
       <c r="BM83" s="5"/>
     </row>
-    <row r="84" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:65">
       <c r="A84" s="4">
         <v>80</v>
       </c>
@@ -8765,7 +8784,7 @@
       <c r="BL84" s="4"/>
       <c r="BM84" s="5"/>
     </row>
-    <row r="85" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:65">
       <c r="A85" s="4">
         <v>81</v>
       </c>
@@ -8846,7 +8865,7 @@
       <c r="BL85" s="4"/>
       <c r="BM85" s="5"/>
     </row>
-    <row r="86" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:65">
       <c r="A86" s="4">
         <v>82</v>
       </c>
@@ -8953,7 +8972,7 @@
       <c r="BL86" s="4"/>
       <c r="BM86" s="5"/>
     </row>
-    <row r="87" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:65">
       <c r="A87" s="4">
         <v>83</v>
       </c>
@@ -9060,7 +9079,7 @@
       <c r="BL87" s="4"/>
       <c r="BM87" s="5"/>
     </row>
-    <row r="88" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:65">
       <c r="A88" s="4">
         <v>84</v>
       </c>
@@ -9145,7 +9164,7 @@
       <c r="BL88" s="4"/>
       <c r="BM88" s="5"/>
     </row>
-    <row r="89" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:65">
       <c r="A89" s="4">
         <v>85</v>
       </c>
@@ -9224,7 +9243,7 @@
       <c r="BL89" s="4"/>
       <c r="BM89" s="5"/>
     </row>
-    <row r="90" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:65">
       <c r="A90" s="4">
         <v>86</v>
       </c>
@@ -9303,7 +9322,7 @@
       <c r="BL90" s="4"/>
       <c r="BM90" s="5"/>
     </row>
-    <row r="91" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:65">
       <c r="A91" s="4">
         <v>87</v>
       </c>
@@ -9390,7 +9409,7 @@
       <c r="BL91" s="4"/>
       <c r="BM91" s="5"/>
     </row>
-    <row r="92" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:65">
       <c r="A92" s="4">
         <v>88</v>
       </c>
@@ -9477,7 +9496,7 @@
       <c r="BL92" s="4"/>
       <c r="BM92" s="5"/>
     </row>
-    <row r="93" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:65">
       <c r="A93" s="4">
         <v>89</v>
       </c>
@@ -9564,7 +9583,7 @@
       <c r="BL93" s="4"/>
       <c r="BM93" s="5"/>
     </row>
-    <row r="94" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:65">
       <c r="A94" s="4">
         <v>90</v>
       </c>
@@ -9651,7 +9670,7 @@
       <c r="BL94" s="4"/>
       <c r="BM94" s="5"/>
     </row>
-    <row r="95" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:65">
       <c r="A95" s="4">
         <v>91</v>
       </c>
@@ -9758,7 +9777,7 @@
       <c r="BL95" s="4"/>
       <c r="BM95" s="5"/>
     </row>
-    <row r="96" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:65">
       <c r="A96" s="4">
         <v>92</v>
       </c>
@@ -9849,7 +9868,7 @@
       <c r="BL96" s="4"/>
       <c r="BM96" s="5"/>
     </row>
-    <row r="97" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:65">
       <c r="A97" s="4">
         <v>93</v>
       </c>
@@ -9956,7 +9975,7 @@
       <c r="BL97" s="4"/>
       <c r="BM97" s="5"/>
     </row>
-    <row r="98" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:65">
       <c r="A98" s="4">
         <v>94</v>
       </c>
@@ -10063,7 +10082,7 @@
       <c r="BL98" s="4"/>
       <c r="BM98" s="5"/>
     </row>
-    <row r="99" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:65">
       <c r="A99" s="4">
         <v>95</v>
       </c>
@@ -10170,7 +10189,7 @@
       <c r="BL99" s="4"/>
       <c r="BM99" s="5"/>
     </row>
-    <row r="100" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:65">
       <c r="A100" s="4">
         <v>96</v>
       </c>
@@ -10277,7 +10296,7 @@
       <c r="BL100" s="4"/>
       <c r="BM100" s="5"/>
     </row>
-    <row r="101" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:65">
       <c r="A101" s="4">
         <v>97</v>
       </c>
@@ -10364,144 +10383,181 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8246CB-5D3A-40C6-9689-10A533CB822C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974DB324-053D-4CBB-BDC5-65D49E568C61}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1">
       <c r="A8" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>236</v>
       </c>
@@ -10513,17 +10569,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3551D49-187C-4829-9BA5-46F59B673A80}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -10533,7 +10589,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -10543,7 +10599,7 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -10553,7 +10609,7 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -10563,7 +10619,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -10573,7 +10629,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -10583,7 +10639,7 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -10593,7 +10649,7 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -10603,7 +10659,7 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -10613,7 +10669,7 @@
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -10623,7 +10679,7 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -10633,7 +10689,7 @@
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -10643,7 +10699,7 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -10653,7 +10709,7 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -10663,7 +10719,7 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -10673,7 +10729,7 @@
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -10683,7 +10739,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -10693,7 +10749,7 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -10703,7 +10759,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -10713,7 +10769,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -10723,7 +10779,7 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -10733,7 +10789,7 @@
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -10743,7 +10799,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -10753,7 +10809,7 @@
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -10763,7 +10819,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -10773,7 +10829,7 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -10783,7 +10839,7 @@
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -10793,7 +10849,7 @@
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -10803,7 +10859,7 @@
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -10813,7 +10869,7 @@
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -10823,7 +10879,7 @@
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -10833,7 +10889,7 @@
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -10843,7 +10899,7 @@
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -10853,7 +10909,7 @@
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -10863,7 +10919,7 @@
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -10873,7 +10929,7 @@
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -10883,7 +10939,7 @@
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -10893,7 +10949,7 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -10903,7 +10959,7 @@
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -10913,7 +10969,7 @@
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -10923,7 +10979,7 @@
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -10933,7 +10989,7 @@
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -10943,7 +10999,7 @@
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -10953,7 +11009,7 @@
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -10963,7 +11019,7 @@
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -10973,7 +11029,7 @@
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -10983,7 +11039,7 @@
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -10993,7 +11049,7 @@
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -11003,7 +11059,7 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -11013,7 +11069,7 @@
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -11023,7 +11079,7 @@
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -11033,7 +11089,7 @@
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -11043,7 +11099,7 @@
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -11053,7 +11109,7 @@
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -11063,7 +11119,7 @@
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -11073,7 +11129,7 @@
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -11083,7 +11139,7 @@
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -11095,6 +11151,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
     <mergeCell ref="B55:D55"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B57:D57"/>
@@ -11111,47 +11208,6 @@
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>